<commit_message>
updated harmonizing by survey
</commit_message>
<xml_diff>
--- a/codebook_combined.xlsx
+++ b/codebook_combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill.sharepoint.com/sites/PROSPERED_Group/Shared Documents/General/CIHR RSBY India/data/Linking code and CSVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1454" documentId="8_{54C3D132-FD60-E343-8A70-19C775275FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F4BC94A-A304-864D-A816-8518F9C038B7}"/>
+  <xr:revisionPtr revIDLastSave="1487" documentId="8_{54C3D132-FD60-E343-8A70-19C775275FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C0A6994-45B3-514C-BB0C-1D8894E67497}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="500" windowWidth="35640" windowHeight="19380" xr2:uid="{73DF8F02-1432-4841-ABC8-0F245F1B77ED}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="35640" windowHeight="19380" xr2:uid="{73DF8F02-1432-4841-ABC8-0F245F1B77ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="646">
   <si>
     <t>Variable</t>
   </si>
@@ -1502,9 +1502,6 @@
   </si>
   <si>
     <t>7 no one</t>
-  </si>
-  <si>
-    <t>NFHS uses an "endorse all" method, so participants can report using a doctor AND an untrained dai. This was recoded to be medical if endorsed any doctor/anm/nurse/midwife/lhv/other health professional, non-medical if dai/TBA/friend/relative/other person, and no one if reported none</t>
   </si>
   <si>
     <t>1 Medical</t>
@@ -1958,6 +1955,33 @@
   </si>
   <si>
     <t xml:space="preserve">14 public tap/standpipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3  tubewell-or-borehole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4   protected-dugwell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           5   unprotected-dug-well</t>
+  </si>
+  <si>
+    <t>6 tanker/truck/cart</t>
+  </si>
+  <si>
+    <t>7other source</t>
+  </si>
+  <si>
+    <t>8 service latrine /dry toilet</t>
+  </si>
+  <si>
+    <t>0 Non-medical</t>
+  </si>
+  <si>
+    <t>Trained dai was recorded as medical, untraine dai as non-medical. For DLHS3 which did not differentiate all dais were recorded as non-medical.</t>
+  </si>
+  <si>
+    <t>not using variable</t>
   </si>
 </sst>
 </file>
@@ -1988,7 +2012,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2017,6 +2041,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2173,7 +2203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2373,6 +2403,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2691,10 +2739,10 @@
   <dimension ref="A1:K198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D163" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I77" sqref="I77"/>
+      <selection pane="bottomRight" activeCell="E181" sqref="E181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2736,7 +2784,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -2759,7 +2807,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2782,7 +2830,7 @@
         <v>420</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2803,10 +2851,10 @@
         <v>421</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2816,7 +2864,7 @@
         <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>366</v>
@@ -2825,10 +2873,10 @@
         <v>422</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2847,10 +2895,10 @@
         <v>423</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2869,10 +2917,10 @@
         <v>424</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2891,10 +2939,10 @@
         <v>425</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2913,10 +2961,10 @@
         <v>426</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2935,10 +2983,10 @@
         <v>427</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2957,10 +3005,10 @@
         <v>428</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2979,7 +3027,7 @@
         <v>429</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2998,7 +3046,7 @@
         <v>430</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3017,7 +3065,7 @@
         <v>431</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3036,7 +3084,7 @@
         <v>432</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3055,7 +3103,7 @@
         <v>433</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3074,7 +3122,7 @@
         <v>434</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3093,7 +3141,7 @@
         <v>435</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3112,7 +3160,7 @@
         <v>436</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3131,7 +3179,7 @@
         <v>437</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3150,7 +3198,7 @@
         <v>438</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3169,7 +3217,7 @@
         <v>439</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3188,7 +3236,7 @@
         <v>440</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3204,7 +3252,7 @@
         <v>441</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3220,7 +3268,7 @@
         <v>442</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3236,7 +3284,7 @@
         <v>443</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3252,7 +3300,7 @@
         <v>444</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3268,7 +3316,7 @@
         <v>445</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3284,7 +3332,7 @@
         <v>446</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3300,7 +3348,7 @@
         <v>447</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3316,7 +3364,7 @@
         <v>448</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3332,7 +3380,7 @@
         <v>449</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3348,7 +3396,7 @@
         <v>450</v>
       </c>
       <c r="I33" s="25" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3364,7 +3412,7 @@
         <v>451</v>
       </c>
       <c r="I34" s="25" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3380,7 +3428,7 @@
         <v>452</v>
       </c>
       <c r="I35" s="25" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3396,7 +3444,7 @@
         <v>453</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3409,7 +3457,7 @@
         <v>399</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3445,143 +3493,143 @@
         <v>455</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H39" s="28" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>560</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="C40" s="17" t="s">
         <v>561</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="D40" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="H40" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="H40" s="12" t="s">
-        <v>563</v>
-      </c>
       <c r="I40" s="30" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="53" t="s">
+        <v>618</v>
+      </c>
+      <c r="B41" s="55" t="s">
         <v>619</v>
       </c>
-      <c r="B41" s="55" t="s">
+      <c r="C41" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>621</v>
-      </c>
       <c r="D41" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H41" s="50"/>
       <c r="I41" s="39" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="59"/>
       <c r="B42" s="63"/>
       <c r="C42" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="H42" s="51"/>
       <c r="I42" s="35" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="59"/>
       <c r="B43" s="63"/>
       <c r="C43" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="H43" s="51"/>
       <c r="I43" s="35" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="54"/>
       <c r="B44" s="56"/>
       <c r="C44" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H44" s="52"/>
       <c r="I44" s="43" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="27" t="s">
+        <v>621</v>
+      </c>
+      <c r="B45" s="26" t="s">
         <v>622</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>623</v>
       </c>
       <c r="C45" s="47"/>
       <c r="D45" s="48"/>
@@ -3590,15 +3638,15 @@
       <c r="G45" s="48"/>
       <c r="H45" s="48"/>
       <c r="I45" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="53" t="s">
+        <v>624</v>
+      </c>
+      <c r="B46" s="55" t="s">
         <v>625</v>
-      </c>
-      <c r="B46" s="55" t="s">
-        <v>626</v>
       </c>
       <c r="C46" s="57"/>
       <c r="D46" s="50"/>
@@ -3637,16 +3685,16 @@
         <v>18</v>
       </c>
       <c r="E48" s="12" t="s">
+        <v>627</v>
+      </c>
+      <c r="F48" s="12" t="s">
         <v>628</v>
       </c>
-      <c r="F48" s="12" t="s">
-        <v>629</v>
-      </c>
       <c r="G48" s="12" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I48" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3672,7 +3720,7 @@
         <v>21</v>
       </c>
       <c r="I49" s="30" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3698,7 +3746,7 @@
         <v>24</v>
       </c>
       <c r="I50" s="30" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3724,7 +3772,7 @@
         <v>25</v>
       </c>
       <c r="I51" s="30" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3750,7 +3798,7 @@
         <v>29</v>
       </c>
       <c r="I52" s="30" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3776,7 +3824,7 @@
         <v>32</v>
       </c>
       <c r="I53" s="31" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3798,7 +3846,7 @@
         <v>33</v>
       </c>
       <c r="I54" s="32" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3953,10 +4001,10 @@
         <v>129</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I61" s="35" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3975,10 +4023,10 @@
         <v>130</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I62" s="35" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3997,7 +4045,7 @@
         <v>131</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4037,7 +4085,7 @@
         <v>259</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4057,7 +4105,7 @@
       </c>
       <c r="G66"/>
       <c r="I66" s="41" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4114,13 +4162,13 @@
         <v>70</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I69" s="31" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4139,10 +4187,10 @@
         <v>136</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I70" s="25" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4161,10 +4209,10 @@
         <v>263</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I71" s="35" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4201,7 +4249,7 @@
         <v>41</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C74" s="17" t="s">
         <v>71</v>
@@ -4216,10 +4264,10 @@
         <v>266</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I74" s="75" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -4293,8 +4341,8 @@
         <v>199</v>
       </c>
       <c r="H77" s="70"/>
-      <c r="I77" s="41" t="s">
-        <v>199</v>
+      <c r="I77" s="38" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4310,14 +4358,14 @@
         <v>313</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>200</v>
       </c>
       <c r="H78" s="70"/>
       <c r="I78" s="38" t="s">
-        <v>200</v>
+        <v>638</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4340,7 +4388,7 @@
       </c>
       <c r="H79" s="70"/>
       <c r="I79" s="38" t="s">
-        <v>201</v>
+        <v>639</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4363,7 +4411,7 @@
       </c>
       <c r="H80" s="70"/>
       <c r="I80" s="38" t="s">
-        <v>202</v>
+        <v>640</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4382,11 +4430,11 @@
         <v>315</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H81" s="70"/>
-      <c r="I81" s="38" t="s">
-        <v>510</v>
+      <c r="I81" s="35" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4405,12 +4453,9 @@
         <v>316</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H82" s="70"/>
-      <c r="I82" s="38" t="s">
-        <v>511</v>
-      </c>
     </row>
     <row r="83" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="59"/>
@@ -4428,12 +4473,9 @@
         <v>317</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H83" s="70"/>
-      <c r="I83" s="35" t="s">
-        <v>512</v>
-      </c>
     </row>
     <row r="84" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="59"/>
@@ -4451,6 +4493,7 @@
         <v>318</v>
       </c>
       <c r="H84" s="70"/>
+      <c r="I84" s="76"/>
     </row>
     <row r="85" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="59"/>
@@ -4468,6 +4511,7 @@
         <v>319</v>
       </c>
       <c r="H85" s="70"/>
+      <c r="I85" s="77"/>
     </row>
     <row r="86" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="59"/>
@@ -4573,10 +4617,10 @@
         <v>325</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I92" s="39" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4595,10 +4639,10 @@
         <v>326</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I93" s="35" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4617,10 +4661,10 @@
         <v>327</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I94" s="35" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4639,10 +4683,10 @@
         <v>328</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I95" s="35" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4661,10 +4705,10 @@
         <v>329</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I96" s="35" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4683,10 +4727,10 @@
         <v>330</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I97" s="35" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4705,10 +4749,10 @@
         <v>331</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I98" s="35" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4727,10 +4771,10 @@
         <v>332</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I99" s="35" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4749,10 +4793,10 @@
         <v>333</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I100" s="35" t="s">
-        <v>521</v>
+        <v>642</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4771,10 +4815,10 @@
         <v>334</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I101" s="35" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4842,10 +4886,10 @@
         <v>83</v>
       </c>
       <c r="G105" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="I105" s="40" t="s">
         <v>574</v>
-      </c>
-      <c r="I105" s="40" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5181,7 +5225,7 @@
       </c>
       <c r="G121" s="5"/>
       <c r="H121" s="73" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I121" s="39" t="s">
         <v>83</v>
@@ -5229,7 +5273,7 @@
       </c>
       <c r="G123" s="5"/>
       <c r="H123" s="69" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I123" s="39" t="s">
         <v>83</v>
@@ -5277,7 +5321,7 @@
       </c>
       <c r="G125" s="12"/>
       <c r="I125" s="30" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="126" spans="1:11" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -5328,7 +5372,7 @@
         <v>181</v>
       </c>
       <c r="I127" s="41" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="128" spans="1:11" s="15" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -5353,7 +5397,7 @@
       <c r="G128" s="12"/>
       <c r="H128" s="12"/>
       <c r="I128" s="42" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="129" spans="1:9" s="15" customFormat="1" ht="68" x14ac:dyDescent="0.2">
@@ -5401,7 +5445,7 @@
       </c>
       <c r="G130" s="5"/>
       <c r="I130" s="31" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5447,7 +5491,7 @@
         <v>269</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H132" s="70"/>
       <c r="I132" s="35" t="s">
@@ -5466,7 +5510,7 @@
       <c r="E133" s="7"/>
       <c r="F133" s="7"/>
       <c r="G133" s="7" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H133" s="71"/>
     </row>
@@ -5490,11 +5534,11 @@
         <v>339</v>
       </c>
       <c r="G134" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H134" s="6"/>
       <c r="I134" s="35" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5513,10 +5557,10 @@
         <v>340</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I135" s="35" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5535,7 +5579,7 @@
         <v>337</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I136" s="1"/>
     </row>
@@ -5555,7 +5599,7 @@
         <v>338</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5574,7 +5618,7 @@
         <v>341</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5593,7 +5637,7 @@
         <v>342</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -5612,7 +5656,7 @@
         <v>343</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5631,7 +5675,7 @@
         <v>344</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5650,7 +5694,7 @@
         <v>345</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -5669,7 +5713,7 @@
         <v>346</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -5688,7 +5732,7 @@
         <v>347</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -5707,7 +5751,7 @@
         <v>348</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5726,7 +5770,7 @@
         <v>349</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5781,19 +5825,19 @@
         <v>477</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H150" s="64" t="s">
-        <v>489</v>
+        <v>644</v>
       </c>
       <c r="I150" s="35" t="s">
-        <v>490</v>
+        <v>643</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5806,17 +5850,17 @@
         <v>478</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H151" s="72"/>
-      <c r="I151" s="35" t="s">
-        <v>491</v>
+      <c r="I151" s="79" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5829,18 +5873,16 @@
         <v>479</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="H152" s="72"/>
-      <c r="I152" s="35" t="s">
-        <v>492</v>
-      </c>
+      <c r="I152" s="78"/>
     </row>
     <row r="153" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="59"/>
@@ -5852,7 +5894,7 @@
         <v>480</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H153" s="72"/>
     </row>
@@ -5866,7 +5908,7 @@
         <v>481</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H154" s="72"/>
     </row>
@@ -5880,7 +5922,7 @@
         <v>482</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H155" s="72"/>
     </row>
@@ -5978,7 +6020,7 @@
       <c r="G160" s="5"/>
       <c r="H160" s="6"/>
       <c r="I160" s="40" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6021,7 +6063,7 @@
       </c>
       <c r="G162" s="12"/>
       <c r="I162" s="40" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="163" spans="1:9" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -6045,7 +6087,7 @@
       </c>
       <c r="G163" s="5"/>
       <c r="I163" s="40" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -6072,7 +6114,7 @@
         <v>4</v>
       </c>
       <c r="I164" s="25" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6117,7 +6159,7 @@
       </c>
       <c r="H166" s="71"/>
       <c r="I166" s="41" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6158,7 +6200,7 @@
         <v>273</v>
       </c>
       <c r="I168" s="41" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6200,8 +6242,8 @@
       </c>
       <c r="G170" s="5"/>
       <c r="H170" s="6"/>
-      <c r="I170" s="39" t="s">
-        <v>83</v>
+      <c r="I170" s="80" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6221,9 +6263,7 @@
       </c>
       <c r="G171" s="7"/>
       <c r="H171" s="8"/>
-      <c r="I171" s="43" t="s">
-        <v>84</v>
-      </c>
+      <c r="I171" s="81"/>
     </row>
     <row r="172" spans="1:9" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="53" t="s">
@@ -6245,7 +6285,7 @@
         <v>350</v>
       </c>
       <c r="G172" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6264,7 +6304,7 @@
         <v>351</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I173" s="44"/>
     </row>
@@ -6284,10 +6324,10 @@
         <v>352</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I174" s="45" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6306,7 +6346,7 @@
         <v>353</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I175" s="44"/>
     </row>
@@ -6326,7 +6366,7 @@
         <v>354</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I176" s="44"/>
     </row>
@@ -6346,7 +6386,7 @@
         <v>355</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I177" s="44"/>
     </row>
@@ -6366,7 +6406,7 @@
         <v>356</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I178" s="44"/>
     </row>
@@ -6386,7 +6426,7 @@
         <v>357</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6405,7 +6445,7 @@
         <v>472</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -6424,7 +6464,7 @@
         <v>359</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6443,7 +6483,7 @@
         <v>469</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -6459,7 +6499,7 @@
         <v>360</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6472,7 +6512,7 @@
         <v>361</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6485,7 +6525,7 @@
         <v>362</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6548,7 +6588,7 @@
         <v>276</v>
       </c>
       <c r="I190" s="41" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="17" x14ac:dyDescent="0.2">

</xml_diff>